<commit_message>
add script for initial amortization amounts
</commit_message>
<xml_diff>
--- a/Data/PlanInfo-UCRP.xlsx
+++ b/Data/PlanInfo-UCRP.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_Main\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_UCRP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,18 @@
     <sheet name="FundingPolicy" sheetId="6" r:id="rId3"/>
     <sheet name="Assumptions" sheetId="3" r:id="rId4"/>
     <sheet name="SalaryGrowth" sheetId="11" r:id="rId5"/>
-    <sheet name="Demo_sum" sheetId="2" r:id="rId6"/>
-    <sheet name="Ret_sum" sheetId="12" r:id="rId7"/>
-    <sheet name="Ret_dec" sheetId="9" r:id="rId8"/>
-    <sheet name="Ret_cashout" sheetId="14" r:id="rId9"/>
-    <sheet name="Ret_bfactor" sheetId="13" r:id="rId10"/>
-    <sheet name="Term_sum" sheetId="15" r:id="rId11"/>
-    <sheet name="Term_dec" sheetId="8" r:id="rId12"/>
-    <sheet name="Disb_sum" sheetId="16" r:id="rId13"/>
-    <sheet name="Disb_dec" sheetId="10" r:id="rId14"/>
-    <sheet name="Death_sum" sheetId="17" r:id="rId15"/>
-    <sheet name="Death_dec" sheetId="5" r:id="rId16"/>
+    <sheet name="Init_amort" sheetId="18" r:id="rId6"/>
+    <sheet name="Demo_sum" sheetId="2" r:id="rId7"/>
+    <sheet name="Ret_sum" sheetId="12" r:id="rId8"/>
+    <sheet name="Ret_dec" sheetId="9" r:id="rId9"/>
+    <sheet name="Ret_cashout" sheetId="14" r:id="rId10"/>
+    <sheet name="Ret_bfactor" sheetId="13" r:id="rId11"/>
+    <sheet name="Term_sum" sheetId="15" r:id="rId12"/>
+    <sheet name="Term_dec" sheetId="8" r:id="rId13"/>
+    <sheet name="Disb_sum" sheetId="16" r:id="rId14"/>
+    <sheet name="Disb_dec" sheetId="10" r:id="rId15"/>
+    <sheet name="Death_sum" sheetId="17" r:id="rId16"/>
+    <sheet name="Death_dec" sheetId="5" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="186">
   <si>
     <t>ppd_id</t>
   </si>
@@ -1938,12 +1939,52 @@
   <si>
     <t>source</t>
   </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Date Established</t>
+  </si>
+  <si>
+    <t>Initial Years</t>
+  </si>
+  <si>
+    <t>Initial Amount</t>
+  </si>
+  <si>
+    <t>Annual Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years remaining </t>
+  </si>
+  <si>
+    <t>Outstanding Balance</t>
+  </si>
+  <si>
+    <t>Actuarial Loss**</t>
+  </si>
+  <si>
+    <t>Actuarial Loss</t>
+  </si>
+  <si>
+    <t>Change in Assumptions</t>
+  </si>
+  <si>
+    <t>Plan Amendment</t>
+  </si>
+  <si>
+    <t>Actuarial Gain</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
@@ -2064,7 +2105,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2205,6 +2246,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2423,6 +2467,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>379898</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>94438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4743450" y="266700"/>
+          <a:ext cx="8819048" cy="6495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -2462,7 +2549,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2543,7 +2630,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2792,6 +2879,49 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>290951</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="3752851"/>
+          <a:ext cx="6901301" cy="3962400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2935,7 +3065,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2978,7 +3108,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3021,7 +3151,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3053,49 +3183,6 @@
         <a:xfrm>
           <a:off x="5086350" y="1200150"/>
           <a:ext cx="7010400" cy="4185751"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>379898</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>94438</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4743450" y="266700"/>
-          <a:ext cx="8819048" cy="6495238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3492,6 +3579,258 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="29" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="D5" s="32">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>6</v>
+      </c>
+      <c r="B6" s="32">
+        <v>0.42</v>
+      </c>
+      <c r="C6" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>7</v>
+      </c>
+      <c r="B7" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>8</v>
+      </c>
+      <c r="B8" s="32">
+        <v>0.35</v>
+      </c>
+      <c r="C8" s="32">
+        <v>0.45</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>9</v>
+      </c>
+      <c r="B9" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0.42</v>
+      </c>
+      <c r="D9" s="32">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>10</v>
+      </c>
+      <c r="B10" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="32">
+        <v>0.42</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>11</v>
+      </c>
+      <c r="B11" s="32">
+        <v>0.18</v>
+      </c>
+      <c r="C11" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>12</v>
+      </c>
+      <c r="B12" s="32">
+        <v>0.16</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>13</v>
+      </c>
+      <c r="B13" s="32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C13" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>14</v>
+      </c>
+      <c r="B14" s="32">
+        <v>0.12</v>
+      </c>
+      <c r="C14" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="32">
+        <v>0.11</v>
+      </c>
+      <c r="C15" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C16" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="32">
+        <v>0.04</v>
+      </c>
+      <c r="C18" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3780,7 +4119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -3920,7 +4259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -4202,7 +4541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4325,7 +4664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -4508,7 +4847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -4601,7 +4940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -4846,7 +5185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -5129,6 +5468,266 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="54">
+        <v>40360</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" s="55">
+        <v>5389886</v>
+      </c>
+      <c r="E4" s="55">
+        <v>416227</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4" s="55">
+        <v>5087113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="54">
+        <v>40725</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5" s="56">
+        <v>905208</v>
+      </c>
+      <c r="E5" s="56">
+        <v>69867</v>
+      </c>
+      <c r="F5">
+        <v>26</v>
+      </c>
+      <c r="G5" s="56">
+        <v>866050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="54">
+        <v>40725</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="56">
+        <v>1513127</v>
+      </c>
+      <c r="E6" s="56">
+        <v>157872</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6" s="56">
+        <v>1253995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="54">
+        <v>40725</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" s="56">
+        <v>-59179</v>
+      </c>
+      <c r="E7" s="56">
+        <v>-6174</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7" s="56">
+        <v>-49044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="54">
+        <v>41091</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8" s="56">
+        <v>2457582</v>
+      </c>
+      <c r="E8" s="56">
+        <v>189587</v>
+      </c>
+      <c r="F8">
+        <v>27</v>
+      </c>
+      <c r="G8" s="56">
+        <v>2380797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="54">
+        <v>41456</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9" s="56">
+        <v>1866282</v>
+      </c>
+      <c r="E9" s="56">
+        <v>143901</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9" s="56">
+        <v>1828830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="54">
+        <v>41821</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" s="56">
+        <v>-886657</v>
+      </c>
+      <c r="E10" s="56">
+        <v>-68334</v>
+      </c>
+      <c r="F10">
+        <v>29</v>
+      </c>
+      <c r="G10" s="56">
+        <v>-878082</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="54">
+        <v>42186</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" s="56">
+        <v>-1440456</v>
+      </c>
+      <c r="E11" s="56">
+        <v>-129251</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11" s="56">
+        <v>-1440456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="54">
+        <v>42186</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" s="56">
+        <v>1850713</v>
+      </c>
+      <c r="E12" s="56">
+        <v>166063</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12" s="56">
+        <v>1850713</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="55">
+        <v>939758</v>
+      </c>
+      <c r="G13" s="55">
+        <v>10899916</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B10"/>
   <sheetViews>
@@ -5187,7 +5786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
@@ -5400,7 +5999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -6070,256 +6669,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="32">
-        <v>0.45</v>
-      </c>
-      <c r="C5" s="32">
-        <v>0.45</v>
-      </c>
-      <c r="D5" s="32">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
-        <v>6</v>
-      </c>
-      <c r="B6" s="32">
-        <v>0.42</v>
-      </c>
-      <c r="C6" s="32">
-        <v>0.45</v>
-      </c>
-      <c r="D6" s="32">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
-        <v>7</v>
-      </c>
-      <c r="B7" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="C7" s="32">
-        <v>0.45</v>
-      </c>
-      <c r="D7" s="32">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>8</v>
-      </c>
-      <c r="B8" s="32">
-        <v>0.35</v>
-      </c>
-      <c r="C8" s="32">
-        <v>0.45</v>
-      </c>
-      <c r="D8" s="32">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
-        <v>9</v>
-      </c>
-      <c r="B9" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="C9" s="32">
-        <v>0.42</v>
-      </c>
-      <c r="D9" s="32">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
-        <v>10</v>
-      </c>
-      <c r="B10" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="C10" s="32">
-        <v>0.42</v>
-      </c>
-      <c r="D10" s="32">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
-        <v>11</v>
-      </c>
-      <c r="B11" s="32">
-        <v>0.18</v>
-      </c>
-      <c r="C11" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="D11" s="32">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
-        <v>12</v>
-      </c>
-      <c r="B12" s="32">
-        <v>0.16</v>
-      </c>
-      <c r="C12" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="D12" s="32">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
-        <v>13</v>
-      </c>
-      <c r="B13" s="32">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="C13" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="D13" s="32">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
-        <v>14</v>
-      </c>
-      <c r="B14" s="32">
-        <v>0.12</v>
-      </c>
-      <c r="C14" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="D14" s="32">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="32">
-        <v>0.11</v>
-      </c>
-      <c r="C15" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="D15" s="32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="32">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C16" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="D16" s="32">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="C17" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="D17" s="32">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="32">
-        <v>0.04</v>
-      </c>
-      <c r="C18" s="32">
-        <v>0.15</v>
-      </c>
-      <c r="D18" s="32">
-        <v>0.04</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
create df for detective work
</commit_message>
<xml_diff>
--- a/Data/PlanInfo-UCRP.xlsx
+++ b/Data/PlanInfo-UCRP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="Death_sum" sheetId="17" r:id="rId16"/>
     <sheet name="Death_dec" sheetId="5" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4298,7 +4298,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5154,8 +5154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5219,8 +5219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5825,7 +5825,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6037,8 +6037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
joint simulation of 3 tiers
</commit_message>
<xml_diff>
--- a/Data/PlanInfo-UCRP.xlsx
+++ b/Data/PlanInfo-UCRP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,20 @@
     <sheet name="Assumptions" sheetId="3" r:id="rId4"/>
     <sheet name="SalaryGrowth" sheetId="11" r:id="rId5"/>
     <sheet name="Init_amort" sheetId="18" r:id="rId6"/>
-    <sheet name="Demo_sum" sheetId="2" r:id="rId7"/>
-    <sheet name="Ret_sum" sheetId="12" r:id="rId8"/>
-    <sheet name="Ret_dec" sheetId="9" r:id="rId9"/>
-    <sheet name="Ret_cashout" sheetId="14" r:id="rId10"/>
-    <sheet name="Ret_bfactor" sheetId="13" r:id="rId11"/>
-    <sheet name="Term_sum" sheetId="15" r:id="rId12"/>
-    <sheet name="Term_dec" sheetId="8" r:id="rId13"/>
-    <sheet name="Disb_sum" sheetId="16" r:id="rId14"/>
-    <sheet name="Disb_dec" sheetId="10" r:id="rId15"/>
-    <sheet name="Death_sum" sheetId="17" r:id="rId16"/>
-    <sheet name="Death_dec" sheetId="5" r:id="rId17"/>
+    <sheet name="External_Funds" sheetId="19" r:id="rId7"/>
+    <sheet name="Demo_sum" sheetId="2" r:id="rId8"/>
+    <sheet name="Ret_sum" sheetId="12" r:id="rId9"/>
+    <sheet name="Ret_dec" sheetId="9" r:id="rId10"/>
+    <sheet name="Ret_cashout" sheetId="14" r:id="rId11"/>
+    <sheet name="Ret_bfactor" sheetId="13" r:id="rId12"/>
+    <sheet name="Term_sum" sheetId="15" r:id="rId13"/>
+    <sheet name="Term_dec" sheetId="8" r:id="rId14"/>
+    <sheet name="Disb_sum" sheetId="16" r:id="rId15"/>
+    <sheet name="Disb_dec" sheetId="10" r:id="rId16"/>
+    <sheet name="Death_sum" sheetId="17" r:id="rId17"/>
+    <sheet name="Death_dec" sheetId="5" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3614,6 +3615,678 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="7" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>51</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="E6" s="33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>52</v>
+      </c>
+      <c r="B7" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="E7" s="33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>53</v>
+      </c>
+      <c r="B8" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="E8" s="33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>54</v>
+      </c>
+      <c r="B9" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>55</v>
+      </c>
+      <c r="B10" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>56</v>
+      </c>
+      <c r="B11" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="33">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G11" s="33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>57</v>
+      </c>
+      <c r="B12" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.06</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="G12" s="33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>58</v>
+      </c>
+      <c r="B13" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="33">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F13" s="33">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G13" s="33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>59</v>
+      </c>
+      <c r="B14" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="G14" s="33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>60</v>
+      </c>
+      <c r="B15" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="F15" s="33">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G15" s="33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>61</v>
+      </c>
+      <c r="B16" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0.16</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0.06</v>
+      </c>
+      <c r="G16" s="33">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>62</v>
+      </c>
+      <c r="B17" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0.18</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0.09</v>
+      </c>
+      <c r="G17" s="33">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>63</v>
+      </c>
+      <c r="B18" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0.18</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>64</v>
+      </c>
+      <c r="B19" s="33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="G19" s="33">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>65</v>
+      </c>
+      <c r="B20" s="33">
+        <v>0.09</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0.4</v>
+      </c>
+      <c r="G20" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>66</v>
+      </c>
+      <c r="B21" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0.13</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0.22</v>
+      </c>
+      <c r="E21" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="G21" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>67</v>
+      </c>
+      <c r="B22" s="33">
+        <v>0.11</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0.22</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0.45</v>
+      </c>
+      <c r="G22" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>68</v>
+      </c>
+      <c r="B23" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0.22</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="F23" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>69</v>
+      </c>
+      <c r="B24" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0.22</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0.22</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="G24" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>70</v>
+      </c>
+      <c r="B25" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="C25" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="G25" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>71</v>
+      </c>
+      <c r="B26" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="C26" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>72</v>
+      </c>
+      <c r="B27" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>73</v>
+      </c>
+      <c r="B28" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="C28" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="D28" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="G28" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>74</v>
+      </c>
+      <c r="B29" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="C29" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="F29" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="G29" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>75</v>
+      </c>
+      <c r="B30" s="33">
+        <v>1</v>
+      </c>
+      <c r="C30" s="33">
+        <v>1</v>
+      </c>
+      <c r="D30" s="33">
+        <v>1</v>
+      </c>
+      <c r="E30" s="33">
+        <v>1</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1</v>
+      </c>
+      <c r="G30" s="33">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3864,7 +4537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
@@ -4154,7 +4827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -4294,7 +4967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -4576,7 +5249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4699,7 +5372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -4882,7 +5555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -4975,7 +5648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -5507,7 +6180,7 @@
   <dimension ref="A3:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD16"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5763,6 +6436,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B10"/>
   <sheetViews>
@@ -5821,11 +6508,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -6032,676 +6719,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="7" width="21.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>50</v>
-      </c>
-      <c r="B5" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="C5" s="33">
-        <v>0</v>
-      </c>
-      <c r="D5" s="33">
-        <v>0.04</v>
-      </c>
-      <c r="E5" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="F5" s="33">
-        <v>0</v>
-      </c>
-      <c r="G5" s="33">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>51</v>
-      </c>
-      <c r="B6" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0</v>
-      </c>
-      <c r="D6" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="E6" s="33">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F6" s="33">
-        <v>0</v>
-      </c>
-      <c r="G6" s="33">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>52</v>
-      </c>
-      <c r="B7" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="C7" s="33">
-        <v>0</v>
-      </c>
-      <c r="D7" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="E7" s="33">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F7" s="33">
-        <v>0</v>
-      </c>
-      <c r="G7" s="33">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>53</v>
-      </c>
-      <c r="B8" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="C8" s="33">
-        <v>0</v>
-      </c>
-      <c r="D8" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="E8" s="33">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F8" s="33">
-        <v>0</v>
-      </c>
-      <c r="G8" s="33">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>54</v>
-      </c>
-      <c r="B9" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="C9" s="33">
-        <v>0</v>
-      </c>
-      <c r="D9" s="33">
-        <v>0.04</v>
-      </c>
-      <c r="E9" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="F9" s="33">
-        <v>0</v>
-      </c>
-      <c r="G9" s="33">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>55</v>
-      </c>
-      <c r="B10" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="C10" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D10" s="33">
-        <v>0.04</v>
-      </c>
-      <c r="E10" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="F10" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="G10" s="33">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>56</v>
-      </c>
-      <c r="B11" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="C11" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="D11" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="E11" s="33">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F11" s="33">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G11" s="33">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>57</v>
-      </c>
-      <c r="B12" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="C12" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="D12" s="33">
-        <v>0.06</v>
-      </c>
-      <c r="E12" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="F12" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="G12" s="33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>58</v>
-      </c>
-      <c r="B13" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="C13" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="D13" s="33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E13" s="33">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F13" s="33">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G13" s="33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>59</v>
-      </c>
-      <c r="B14" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="C14" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="D14" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="E14" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="F14" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="G14" s="33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>60</v>
-      </c>
-      <c r="B15" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="C15" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D15" s="33">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E15" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="F15" s="33">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G15" s="33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>61</v>
-      </c>
-      <c r="B16" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="C16" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D16" s="33">
-        <v>0.16</v>
-      </c>
-      <c r="E16" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="33">
-        <v>0.06</v>
-      </c>
-      <c r="G16" s="33">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>62</v>
-      </c>
-      <c r="B17" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="C17" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D17" s="33">
-        <v>0.18</v>
-      </c>
-      <c r="E17" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="F17" s="33">
-        <v>0.09</v>
-      </c>
-      <c r="G17" s="33">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>63</v>
-      </c>
-      <c r="B18" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="C18" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D18" s="33">
-        <v>0.18</v>
-      </c>
-      <c r="E18" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="F18" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="G18" s="33">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>64</v>
-      </c>
-      <c r="B19" s="33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C19" s="33">
-        <v>0.03</v>
-      </c>
-      <c r="D19" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="E19" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="F19" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="G19" s="33">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>65</v>
-      </c>
-      <c r="B20" s="33">
-        <v>0.09</v>
-      </c>
-      <c r="C20" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="D20" s="33">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="33">
-        <v>0.4</v>
-      </c>
-      <c r="F20" s="33">
-        <v>0.4</v>
-      </c>
-      <c r="G20" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>66</v>
-      </c>
-      <c r="B21" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="C21" s="33">
-        <v>0.13</v>
-      </c>
-      <c r="D21" s="33">
-        <v>0.22</v>
-      </c>
-      <c r="E21" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="F21" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="G21" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>67</v>
-      </c>
-      <c r="B22" s="33">
-        <v>0.11</v>
-      </c>
-      <c r="C22" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="D22" s="33">
-        <v>0.22</v>
-      </c>
-      <c r="E22" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="F22" s="33">
-        <v>0.45</v>
-      </c>
-      <c r="G22" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>68</v>
-      </c>
-      <c r="B23" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="C23" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="D23" s="33">
-        <v>0.22</v>
-      </c>
-      <c r="E23" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="F23" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="G23" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>69</v>
-      </c>
-      <c r="B24" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="C24" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="D24" s="33">
-        <v>0.22</v>
-      </c>
-      <c r="E24" s="33">
-        <v>0.22</v>
-      </c>
-      <c r="F24" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="G24" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>70</v>
-      </c>
-      <c r="B25" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="C25" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="D25" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="F25" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="G25" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>71</v>
-      </c>
-      <c r="B26" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="C26" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="D26" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="E26" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="F26" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="G26" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>72</v>
-      </c>
-      <c r="B27" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="C27" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="D27" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="E27" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="F27" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="G27" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>73</v>
-      </c>
-      <c r="B28" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="C28" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="D28" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="E28" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="F28" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="G28" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>74</v>
-      </c>
-      <c r="B29" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="C29" s="33">
-        <v>0.12</v>
-      </c>
-      <c r="D29" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="E29" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="F29" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="G29" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>75</v>
-      </c>
-      <c r="B30" s="33">
-        <v>1</v>
-      </c>
-      <c r="C30" s="33">
-        <v>1</v>
-      </c>
-      <c r="D30" s="33">
-        <v>1</v>
-      </c>
-      <c r="E30" s="33">
-        <v>1</v>
-      </c>
-      <c r="F30" s="33">
-        <v>1</v>
-      </c>
-      <c r="G30" s="33">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>